<commit_message>
Adding MB 2014 manual sonde cast data and updating script to include these data
</commit_message>
<xml_diff>
--- a/01_raw data/2014_Manual_Sonde_Casts.xlsx
+++ b/01_raw data/2014_Manual_Sonde_Casts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinkincaid/ownCloud/bree_frozeN/01_raw data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBFFEE25-3C52-4A4D-937C-691AB6CD2A63}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C5AF90-B9A8-5141-B253-35C140097C6C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="840" windowWidth="28200" windowHeight="21860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2560" yWindow="840" windowWidth="31120" windowHeight="21860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All winter" sheetId="24" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="168">
   <si>
     <t>DateTime</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>MAIN2013.DAT</t>
-  </si>
-  <si>
-    <t>NOTES</t>
   </si>
   <si>
     <t>MAIN13B.DAT</t>
@@ -993,9 +990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A1A403-6B98-E249-87E8-2E96DF31FB04}">
   <dimension ref="A1:P238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1023,16 +1018,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>5</v>
@@ -1044,22 +1039,22 @@
         <v>7</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>167</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>168</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>24</v>
@@ -3828,8 +3823,8 @@
       <c r="D57" s="6">
         <v>0.159</v>
       </c>
-      <c r="E57" s="6">
-        <v>128</v>
+      <c r="E57">
+        <v>0.128</v>
       </c>
       <c r="F57" s="6">
         <v>3.4000000000000002E-2</v>
@@ -3862,7 +3857,7 @@
         <v>1.4</v>
       </c>
       <c r="P57" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
@@ -3878,8 +3873,8 @@
       <c r="D58" s="6">
         <v>0.159</v>
       </c>
-      <c r="E58" s="6">
-        <v>128</v>
+      <c r="E58">
+        <v>0.128</v>
       </c>
       <c r="F58" s="6">
         <v>5.1999999999999998E-2</v>
@@ -3912,7 +3907,7 @@
         <v>1.6</v>
       </c>
       <c r="P58" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
@@ -3928,8 +3923,8 @@
       <c r="D59" s="6">
         <v>0.159</v>
       </c>
-      <c r="E59" s="6">
-        <v>128</v>
+      <c r="E59">
+        <v>0.128</v>
       </c>
       <c r="F59" s="6">
         <v>1.4999999999999999E-2</v>
@@ -3962,7 +3957,7 @@
         <v>1.4</v>
       </c>
       <c r="P59" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
@@ -3978,8 +3973,8 @@
       <c r="D60" s="6">
         <v>0.159</v>
       </c>
-      <c r="E60" s="6">
-        <v>127</v>
+      <c r="E60">
+        <v>0.127</v>
       </c>
       <c r="F60" s="6">
         <v>0.51100000000000001</v>
@@ -4012,7 +4007,7 @@
         <v>1.8</v>
       </c>
       <c r="P60" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
@@ -4028,8 +4023,8 @@
       <c r="D61" s="6">
         <v>0.159</v>
       </c>
-      <c r="E61" s="6">
-        <v>127</v>
+      <c r="E61">
+        <v>0.127</v>
       </c>
       <c r="F61" s="6">
         <v>0.495</v>
@@ -4062,7 +4057,7 @@
         <v>1.7</v>
       </c>
       <c r="P61" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
@@ -4078,8 +4073,8 @@
       <c r="D62" s="6">
         <v>0.159</v>
       </c>
-      <c r="E62" s="6">
-        <v>127</v>
+      <c r="E62">
+        <v>0.127</v>
       </c>
       <c r="F62" s="6">
         <v>0.47699999999999998</v>
@@ -4112,7 +4107,7 @@
         <v>1.6</v>
       </c>
       <c r="P62" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
@@ -4128,8 +4123,8 @@
       <c r="D63" s="6">
         <v>0.159</v>
       </c>
-      <c r="E63" s="6">
-        <v>127</v>
+      <c r="E63">
+        <v>0.127</v>
       </c>
       <c r="F63" s="6">
         <v>0.99199999999999999</v>
@@ -4162,7 +4157,7 @@
         <v>1.6</v>
       </c>
       <c r="P63" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
@@ -4178,8 +4173,8 @@
       <c r="D64" s="6">
         <v>0.158</v>
       </c>
-      <c r="E64" s="6">
-        <v>127</v>
+      <c r="E64">
+        <v>0.127</v>
       </c>
       <c r="F64" s="6">
         <v>0.98899999999999999</v>
@@ -4212,7 +4207,7 @@
         <v>1.6</v>
       </c>
       <c r="P64" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
@@ -4228,8 +4223,8 @@
       <c r="D65" s="6">
         <v>0.158</v>
       </c>
-      <c r="E65" s="6">
-        <v>127</v>
+      <c r="E65">
+        <v>0.127</v>
       </c>
       <c r="F65" s="6">
         <v>0.99399999999999999</v>
@@ -4262,7 +4257,7 @@
         <v>1.6</v>
       </c>
       <c r="P65" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
@@ -4278,8 +4273,8 @@
       <c r="D66" s="6">
         <v>0.159</v>
       </c>
-      <c r="E66" s="6">
-        <v>127</v>
+      <c r="E66">
+        <v>0.127</v>
       </c>
       <c r="F66" s="6">
         <v>1.4950000000000001</v>
@@ -4312,7 +4307,7 @@
         <v>1.7</v>
       </c>
       <c r="P66" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
@@ -4328,8 +4323,8 @@
       <c r="D67" s="6">
         <v>0.158</v>
       </c>
-      <c r="E67" s="6">
-        <v>127</v>
+      <c r="E67">
+        <v>0.127</v>
       </c>
       <c r="F67" s="6">
         <v>1.5049999999999999</v>
@@ -4362,7 +4357,7 @@
         <v>1.8</v>
       </c>
       <c r="P67" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
@@ -4378,8 +4373,8 @@
       <c r="D68" s="6">
         <v>0.158</v>
       </c>
-      <c r="E68" s="6">
-        <v>126</v>
+      <c r="E68">
+        <v>0.126</v>
       </c>
       <c r="F68" s="6">
         <v>1.4990000000000001</v>
@@ -4412,7 +4407,7 @@
         <v>1.9</v>
       </c>
       <c r="P68" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
@@ -4428,8 +4423,8 @@
       <c r="D69" s="6">
         <v>0.159</v>
       </c>
-      <c r="E69" s="6">
-        <v>127</v>
+      <c r="E69">
+        <v>0.127</v>
       </c>
       <c r="F69" s="6">
         <v>2.0049999999999999</v>
@@ -4462,7 +4457,7 @@
         <v>1.7</v>
       </c>
       <c r="P69" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
@@ -4478,8 +4473,8 @@
       <c r="D70" s="6">
         <v>0.158</v>
       </c>
-      <c r="E70" s="6">
-        <v>126</v>
+      <c r="E70">
+        <v>0.126</v>
       </c>
       <c r="F70" s="6">
         <v>2.0099999999999998</v>
@@ -4512,7 +4507,7 @@
         <v>1.6</v>
       </c>
       <c r="P70" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
@@ -4528,8 +4523,8 @@
       <c r="D71" s="6">
         <v>0.159</v>
       </c>
-      <c r="E71" s="6">
-        <v>127</v>
+      <c r="E71">
+        <v>0.127</v>
       </c>
       <c r="F71" s="6">
         <v>2.008</v>
@@ -4562,7 +4557,7 @@
         <v>1.6</v>
       </c>
       <c r="P71" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
@@ -4578,8 +4573,8 @@
       <c r="D72" s="6">
         <v>0.159</v>
       </c>
-      <c r="E72" s="6">
-        <v>127</v>
+      <c r="E72">
+        <v>0.127</v>
       </c>
       <c r="F72" s="6">
         <v>2.4969999999999999</v>
@@ -4612,7 +4607,7 @@
         <v>1.7</v>
       </c>
       <c r="P72" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
@@ -4628,8 +4623,8 @@
       <c r="D73" s="6">
         <v>0.159</v>
       </c>
-      <c r="E73" s="6">
-        <v>127</v>
+      <c r="E73">
+        <v>0.127</v>
       </c>
       <c r="F73" s="6">
         <v>2.4950000000000001</v>
@@ -4662,7 +4657,7 @@
         <v>1.7</v>
       </c>
       <c r="P73" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
@@ -4678,8 +4673,8 @@
       <c r="D74" s="6">
         <v>0.159</v>
       </c>
-      <c r="E74" s="6">
-        <v>127</v>
+      <c r="E74">
+        <v>0.127</v>
       </c>
       <c r="F74" s="6">
         <v>2.496</v>
@@ -4712,7 +4707,7 @@
         <v>1.7</v>
       </c>
       <c r="P74" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
@@ -12471,154 +12466,154 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
         <v>73</v>
-      </c>
-      <c r="B5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
         <v>76</v>
-      </c>
-      <c r="B7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
         <v>78</v>
-      </c>
-      <c r="B8" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
         <v>80</v>
-      </c>
-      <c r="B9" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
         <v>82</v>
-      </c>
-      <c r="B10" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
         <v>85</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>86</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>87</v>
-      </c>
-      <c r="D13" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" t="s">
         <v>89</v>
-      </c>
-      <c r="D14" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
         <v>91</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>92</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>93</v>
-      </c>
-      <c r="D15" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" t="s">
         <v>95</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>96</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>97</v>
-      </c>
-      <c r="D16" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" t="s">
         <v>99</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" t="s">
         <v>100</v>
-      </c>
-      <c r="C17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" t="s">
         <v>102</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" t="s">
         <v>103</v>
-      </c>
-      <c r="C18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" t="s">
         <v>105</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" t="s">
         <v>106</v>
-      </c>
-      <c r="C19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
@@ -12626,66 +12621,66 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" t="s">
         <v>108</v>
-      </c>
-      <c r="C20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" t="s">
         <v>110</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" t="s">
         <v>111</v>
-      </c>
-      <c r="C21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" t="s">
         <v>113</v>
       </c>
-      <c r="B22" t="s">
-        <v>114</v>
-      </c>
       <c r="C22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" t="s">
         <v>115</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" t="s">
         <v>116</v>
       </c>
-      <c r="C23" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="S23" t="s">
         <v>117</v>
-      </c>
-      <c r="S23" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" t="s">
         <v>119</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>120</v>
-      </c>
-      <c r="C24" t="s">
-        <v>121</v>
       </c>
       <c r="D24">
         <v>19</v>
@@ -12750,10 +12745,10 @@
         <v>18</v>
       </c>
       <c r="S26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T26" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U26">
         <v>19</v>
@@ -12791,97 +12786,97 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" t="s">
         <v>123</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>124</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>125</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>126</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>127</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>128</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>129</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>130</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>131</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>132</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>133</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>134</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>135</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>136</v>
-      </c>
-      <c r="O27" t="s">
-        <v>137</v>
       </c>
       <c r="P27" t="s">
         <v>5</v>
       </c>
       <c r="Q27" t="s">
+        <v>137</v>
+      </c>
+      <c r="R27" t="s">
         <v>138</v>
       </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>139</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="T27" s="5" t="s">
+      <c r="U27" t="s">
         <v>141</v>
       </c>
-      <c r="U27" t="s">
+      <c r="V27" t="s">
         <v>142</v>
       </c>
-      <c r="V27" t="s">
+      <c r="W27" t="s">
         <v>143</v>
       </c>
-      <c r="W27" t="s">
+      <c r="X27" t="s">
         <v>144</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Y27" t="s">
         <v>145</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="Z27" t="s">
         <v>146</v>
       </c>
-      <c r="Z27" t="s">
+      <c r="AA27" t="s">
         <v>147</v>
       </c>
-      <c r="AA27" t="s">
+      <c r="AB27" t="s">
         <v>148</v>
       </c>
-      <c r="AB27" t="s">
+      <c r="AC27" t="s">
         <v>149</v>
       </c>
-      <c r="AC27" t="s">
+      <c r="AD27" t="s">
         <v>150</v>
       </c>
-      <c r="AD27" t="s">
+      <c r="AE27" t="s">
         <v>151</v>
-      </c>
-      <c r="AE27" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
@@ -12895,7 +12890,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -12992,7 +12987,7 @@
         <v>0.443</v>
       </c>
       <c r="D29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -13089,7 +13084,7 @@
         <v>0.73</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -13186,7 +13181,7 @@
         <v>0.23799999999999999</v>
       </c>
       <c r="D31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -13283,7 +13278,7 @@
         <v>0.80700000000000005</v>
       </c>
       <c r="D32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -13380,7 +13375,7 @@
         <v>0.67</v>
       </c>
       <c r="D33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -13477,7 +13472,7 @@
         <v>0.66200000000000003</v>
       </c>
       <c r="D34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -13574,7 +13569,7 @@
         <v>0.22600000000000001</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -13671,7 +13666,7 @@
         <v>0.40600000000000003</v>
       </c>
       <c r="D36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -13768,7 +13763,7 @@
         <v>0.58899999999999997</v>
       </c>
       <c r="D37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -13865,7 +13860,7 @@
         <v>0.246</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -13962,7 +13957,7 @@
         <v>0.42499999999999999</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -14059,7 +14054,7 @@
         <v>0.23</v>
       </c>
       <c r="D40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -14156,7 +14151,7 @@
         <v>0.48099999999999998</v>
       </c>
       <c r="D41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -14253,7 +14248,7 @@
         <v>0.52</v>
       </c>
       <c r="D42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -14350,7 +14345,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="D43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -14447,7 +14442,7 @@
         <v>0.64500000000000002</v>
       </c>
       <c r="D44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -14544,7 +14539,7 @@
         <v>0.36299999999999999</v>
       </c>
       <c r="D45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -14641,7 +14636,7 @@
         <v>0.68300000000000005</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -14738,7 +14733,7 @@
         <v>0.28699999999999998</v>
       </c>
       <c r="D47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -14835,7 +14830,7 @@
         <v>0.52100000000000002</v>
       </c>
       <c r="D48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -14932,7 +14927,7 @@
         <v>0.41199999999999998</v>
       </c>
       <c r="D49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -15029,7 +15024,7 @@
         <v>0.44700000000000001</v>
       </c>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -15126,7 +15121,7 @@
         <v>0.14799999999999999</v>
       </c>
       <c r="D51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -15223,7 +15218,7 @@
         <v>0.94</v>
       </c>
       <c r="D52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -15320,7 +15315,7 @@
         <v>0.68899999999999995</v>
       </c>
       <c r="D53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -15417,7 +15412,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="D54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -15514,7 +15509,7 @@
         <v>0.88900000000000001</v>
       </c>
       <c r="D55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -15611,7 +15606,7 @@
         <v>0.42799999999999999</v>
       </c>
       <c r="D56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -15708,7 +15703,7 @@
         <v>0.34399999999999997</v>
       </c>
       <c r="D57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -15805,7 +15800,7 @@
         <v>0.52600000000000002</v>
       </c>
       <c r="D58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -15902,7 +15897,7 @@
         <v>0.17100000000000001</v>
       </c>
       <c r="D59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -16035,154 +16030,154 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
         <v>73</v>
-      </c>
-      <c r="B5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
         <v>76</v>
-      </c>
-      <c r="B7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
         <v>78</v>
-      </c>
-      <c r="B8" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
         <v>80</v>
-      </c>
-      <c r="B9" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
         <v>82</v>
-      </c>
-      <c r="B10" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
         <v>85</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>86</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>87</v>
-      </c>
-      <c r="D13" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" t="s">
         <v>89</v>
-      </c>
-      <c r="D14" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
         <v>91</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>92</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>93</v>
-      </c>
-      <c r="D15" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" t="s">
         <v>95</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>96</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>97</v>
-      </c>
-      <c r="D16" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" t="s">
         <v>99</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" t="s">
         <v>100</v>
-      </c>
-      <c r="C17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" t="s">
         <v>102</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" t="s">
         <v>103</v>
-      </c>
-      <c r="C18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" t="s">
         <v>105</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" t="s">
         <v>106</v>
-      </c>
-      <c r="C19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.2">
@@ -16190,67 +16185,67 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" t="s">
         <v>108</v>
-      </c>
-      <c r="C20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" t="s">
         <v>110</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" t="s">
         <v>111</v>
-      </c>
-      <c r="C21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" t="s">
         <v>113</v>
       </c>
-      <c r="B22" t="s">
-        <v>114</v>
-      </c>
       <c r="C22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" t="s">
         <v>115</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" t="s">
         <v>116</v>
       </c>
-      <c r="C23" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="S23" t="s">
         <v>117</v>
-      </c>
-      <c r="S23" t="s">
-        <v>118</v>
       </c>
       <c r="T23" s="5"/>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" t="s">
         <v>119</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>120</v>
-      </c>
-      <c r="C24" t="s">
-        <v>121</v>
       </c>
       <c r="D24">
         <v>19</v>
@@ -16319,10 +16314,10 @@
         <v>18</v>
       </c>
       <c r="S26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T26" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U26">
         <v>19</v>
@@ -16360,100 +16355,100 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" t="s">
         <v>123</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>124</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>125</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>126</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>127</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>128</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>129</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>130</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>131</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>132</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>133</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>134</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>135</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>136</v>
-      </c>
-      <c r="O27" t="s">
-        <v>137</v>
       </c>
       <c r="P27" t="s">
         <v>5</v>
       </c>
       <c r="Q27" t="s">
+        <v>137</v>
+      </c>
+      <c r="R27" t="s">
         <v>138</v>
       </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>139</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="T27" s="5" t="s">
+      <c r="U27" t="s">
         <v>141</v>
       </c>
-      <c r="U27" t="s">
+      <c r="V27" t="s">
         <v>142</v>
       </c>
-      <c r="V27" t="s">
+      <c r="W27" t="s">
         <v>143</v>
       </c>
-      <c r="W27" t="s">
+      <c r="X27" t="s">
         <v>144</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Y27" t="s">
         <v>145</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="Z27" t="s">
         <v>146</v>
       </c>
-      <c r="Z27" t="s">
+      <c r="AA27" t="s">
         <v>147</v>
       </c>
-      <c r="AA27" t="s">
+      <c r="AB27" t="s">
         <v>148</v>
       </c>
-      <c r="AB27" t="s">
+      <c r="AC27" t="s">
         <v>149</v>
       </c>
-      <c r="AC27" t="s">
+      <c r="AD27" t="s">
         <v>150</v>
       </c>
-      <c r="AD27" t="s">
+      <c r="AE27" t="s">
         <v>151</v>
       </c>
-      <c r="AE27" t="s">
-        <v>152</v>
-      </c>
       <c r="AF27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.2">
@@ -16467,7 +16462,7 @@
         <v>0.42399999999999999</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -16553,7 +16548,7 @@
         <v>4.5</v>
       </c>
       <c r="AF28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.2">
@@ -16567,7 +16562,7 @@
         <v>0.05</v>
       </c>
       <c r="D29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -16653,7 +16648,7 @@
         <v>4.5</v>
       </c>
       <c r="AF29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.2">
@@ -16667,7 +16662,7 @@
         <v>0.501</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -16753,7 +16748,7 @@
         <v>4.5</v>
       </c>
       <c r="AF30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.2">
@@ -16767,7 +16762,7 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="D31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -16853,7 +16848,7 @@
         <v>4.5</v>
       </c>
       <c r="AF31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.2">
@@ -16867,7 +16862,7 @@
         <v>0.95399999999999996</v>
       </c>
       <c r="D32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -16953,7 +16948,7 @@
         <v>4.5</v>
       </c>
       <c r="AF32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.2">
@@ -16967,7 +16962,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="D33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -17053,7 +17048,7 @@
         <v>4.5</v>
       </c>
       <c r="AF33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.2">
@@ -17067,7 +17062,7 @@
         <v>0.33300000000000002</v>
       </c>
       <c r="D34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -17153,7 +17148,7 @@
         <v>4.5</v>
       </c>
       <c r="AF34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.2">
@@ -17167,7 +17162,7 @@
         <v>0.44500000000000001</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -17253,7 +17248,7 @@
         <v>4.5</v>
       </c>
       <c r="AF35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.2">
@@ -17267,7 +17262,7 @@
         <v>0.55900000000000005</v>
       </c>
       <c r="D36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -17353,7 +17348,7 @@
         <v>4.5</v>
       </c>
       <c r="AF36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:32" x14ac:dyDescent="0.2">
@@ -17367,7 +17362,7 @@
         <v>9.4E-2</v>
       </c>
       <c r="D37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -17453,7 +17448,7 @@
         <v>4.5</v>
       </c>
       <c r="AF37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:32" x14ac:dyDescent="0.2">
@@ -17467,7 +17462,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -17553,7 +17548,7 @@
         <v>4.5</v>
       </c>
       <c r="AF38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:32" x14ac:dyDescent="0.2">
@@ -17567,7 +17562,7 @@
         <v>0.84299999999999997</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -17653,7 +17648,7 @@
         <v>4.5</v>
       </c>
       <c r="AF39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:32" x14ac:dyDescent="0.2">
@@ -17667,7 +17662,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="D40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -17753,7 +17748,7 @@
         <v>4.5</v>
       </c>
       <c r="AF40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.2">
@@ -17767,7 +17762,7 @@
         <v>0.996</v>
       </c>
       <c r="D41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -17853,7 +17848,7 @@
         <v>4.5</v>
       </c>
       <c r="AF41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:32" x14ac:dyDescent="0.2">
@@ -17867,7 +17862,7 @@
         <v>0.9</v>
       </c>
       <c r="D42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -17953,7 +17948,7 @@
         <v>4.5</v>
       </c>
       <c r="AF42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.2">
@@ -17967,7 +17962,7 @@
         <v>0.71699999999999997</v>
       </c>
       <c r="D43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -18053,7 +18048,7 @@
         <v>4.5</v>
       </c>
       <c r="AF43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.2">
@@ -18067,7 +18062,7 @@
         <v>0.38600000000000001</v>
       </c>
       <c r="D44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -18153,7 +18148,7 @@
         <v>4.5</v>
       </c>
       <c r="AF44" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.2">
@@ -18167,7 +18162,7 @@
         <v>0.245</v>
       </c>
       <c r="D45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -18253,7 +18248,7 @@
         <v>4.5</v>
       </c>
       <c r="AF45" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.2">
@@ -18267,7 +18262,7 @@
         <v>0.89</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -18353,7 +18348,7 @@
         <v>4.5</v>
       </c>
       <c r="AF46" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.2">
@@ -18367,7 +18362,7 @@
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="D47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -18453,7 +18448,7 @@
         <v>4.5</v>
       </c>
       <c r="AF47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.2">
@@ -18467,7 +18462,7 @@
         <v>0.93200000000000005</v>
       </c>
       <c r="D48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -18553,7 +18548,7 @@
         <v>4.5</v>
       </c>
       <c r="AF48" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:32" x14ac:dyDescent="0.2">
@@ -18567,7 +18562,7 @@
         <v>0.64</v>
       </c>
       <c r="D49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -18653,7 +18648,7 @@
         <v>4.5</v>
       </c>
       <c r="AF49" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="50" spans="1:32" x14ac:dyDescent="0.2">
@@ -18667,7 +18662,7 @@
         <v>0.59499999999999997</v>
       </c>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -18753,7 +18748,7 @@
         <v>4.5</v>
       </c>
       <c r="AF50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:32" x14ac:dyDescent="0.2">
@@ -18767,7 +18762,7 @@
         <v>0.42399999999999999</v>
       </c>
       <c r="D51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -18853,7 +18848,7 @@
         <v>4.5</v>
       </c>
       <c r="AF51" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:32" x14ac:dyDescent="0.2">
@@ -18867,7 +18862,7 @@
         <v>0.372</v>
       </c>
       <c r="D52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -18953,7 +18948,7 @@
         <v>4.5</v>
       </c>
       <c r="AF52" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:32" x14ac:dyDescent="0.2">
@@ -18967,7 +18962,7 @@
         <v>0.55600000000000005</v>
       </c>
       <c r="D53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -19053,7 +19048,7 @@
         <v>4.5</v>
       </c>
       <c r="AF53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.2">
@@ -19067,7 +19062,7 @@
         <v>0.373</v>
       </c>
       <c r="D54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -19153,7 +19148,7 @@
         <v>4.5</v>
       </c>
       <c r="AF54" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:32" x14ac:dyDescent="0.2">
@@ -19167,7 +19162,7 @@
         <v>9.4E-2</v>
       </c>
       <c r="D55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -19253,7 +19248,7 @@
         <v>4.5</v>
       </c>
       <c r="AF55" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:32" x14ac:dyDescent="0.2">
@@ -19267,7 +19262,7 @@
         <v>0.98</v>
       </c>
       <c r="D56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -19353,7 +19348,7 @@
         <v>4.5</v>
       </c>
       <c r="AF56" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:32" x14ac:dyDescent="0.2">
@@ -19367,7 +19362,7 @@
         <v>0.69799999999999995</v>
       </c>
       <c r="D57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -19453,7 +19448,7 @@
         <v>4.5</v>
       </c>
       <c r="AF57" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:32" x14ac:dyDescent="0.2">
@@ -19467,7 +19462,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="D58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -19553,7 +19548,7 @@
         <v>4.5</v>
       </c>
       <c r="AF58" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:32" x14ac:dyDescent="0.2">
@@ -19567,7 +19562,7 @@
         <v>0.50600000000000001</v>
       </c>
       <c r="D59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -19653,7 +19648,7 @@
         <v>4.5</v>
       </c>
       <c r="AF59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:32" x14ac:dyDescent="0.2">
@@ -19667,7 +19662,7 @@
         <v>0.41099999999999998</v>
       </c>
       <c r="D60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -19753,7 +19748,7 @@
         <v>4.5</v>
       </c>
       <c r="AF60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.2">
@@ -19767,7 +19762,7 @@
         <v>0.66500000000000004</v>
       </c>
       <c r="D61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -19853,7 +19848,7 @@
         <v>4.5</v>
       </c>
       <c r="AF61" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:32" x14ac:dyDescent="0.2">
@@ -19867,7 +19862,7 @@
         <v>0.41699999999999998</v>
       </c>
       <c r="D62" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -19953,7 +19948,7 @@
         <v>4.5</v>
       </c>
       <c r="AF62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="63" spans="1:32" x14ac:dyDescent="0.2">
@@ -19967,7 +19962,7 @@
         <v>0.29199999999999998</v>
       </c>
       <c r="D63" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -20053,7 +20048,7 @@
         <v>4.5</v>
       </c>
       <c r="AF63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:32" x14ac:dyDescent="0.2">
@@ -20067,7 +20062,7 @@
         <v>0.91500000000000004</v>
       </c>
       <c r="D64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -20153,7 +20148,7 @@
         <v>4.5</v>
       </c>
       <c r="AF64" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="65" spans="1:32" x14ac:dyDescent="0.2">
@@ -20167,7 +20162,7 @@
         <v>0.68799999999999994</v>
       </c>
       <c r="D65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -20253,7 +20248,7 @@
         <v>4.5</v>
       </c>
       <c r="AF65" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -20332,7 +20327,7 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -26209,7 +26204,7 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -26239,7 +26234,7 @@
         <v>23</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -27579,7 +27574,7 @@
         <v>12</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -29224,7 +29219,7 @@
         <v>12</v>
       </c>
       <c r="Q1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R1" t="s">
         <v>4</v>
@@ -29244,7 +29239,7 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -29256,7 +29251,7 @@
         <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K2" t="s">
         <v>19</v>
@@ -29277,10 +29272,10 @@
         <v>23</v>
       </c>
       <c r="Q2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" t="s">
         <v>32</v>
-      </c>
-      <c r="R2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -31778,20 +31773,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q75"/>
+  <dimension ref="A1:P75"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58:E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="86.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -31835,7 +31829,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -31881,11 +31875,8 @@
       <c r="P2" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -31935,7 +31926,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -31985,7 +31976,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -32035,7 +32026,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -32085,7 +32076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -32135,7 +32126,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -32185,7 +32176,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -32235,7 +32226,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -32285,7 +32276,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -32335,7 +32326,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -32385,7 +32376,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -32435,7 +32426,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -32485,7 +32476,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -32535,7 +32526,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
@@ -34649,7 +34640,7 @@
         <v>0.159</v>
       </c>
       <c r="E58">
-        <v>128</v>
+        <v>0.128</v>
       </c>
       <c r="F58">
         <v>3.4000000000000002E-2</v>
@@ -34682,7 +34673,7 @@
         <v>1.4</v>
       </c>
       <c r="P58" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
@@ -34699,7 +34690,7 @@
         <v>0.159</v>
       </c>
       <c r="E59">
-        <v>128</v>
+        <v>0.128</v>
       </c>
       <c r="F59">
         <v>5.1999999999999998E-2</v>
@@ -34732,7 +34723,7 @@
         <v>1.6</v>
       </c>
       <c r="P59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
@@ -34749,7 +34740,7 @@
         <v>0.159</v>
       </c>
       <c r="E60">
-        <v>128</v>
+        <v>0.128</v>
       </c>
       <c r="F60">
         <v>1.4999999999999999E-2</v>
@@ -34782,7 +34773,7 @@
         <v>1.4</v>
       </c>
       <c r="P60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
@@ -34799,7 +34790,7 @@
         <v>0.159</v>
       </c>
       <c r="E61">
-        <v>127</v>
+        <v>0.127</v>
       </c>
       <c r="F61">
         <v>0.51100000000000001</v>
@@ -34832,7 +34823,7 @@
         <v>1.8</v>
       </c>
       <c r="P61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
@@ -34849,7 +34840,7 @@
         <v>0.159</v>
       </c>
       <c r="E62">
-        <v>127</v>
+        <v>0.127</v>
       </c>
       <c r="F62">
         <v>0.495</v>
@@ -34882,7 +34873,7 @@
         <v>1.7</v>
       </c>
       <c r="P62" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
@@ -34899,7 +34890,7 @@
         <v>0.159</v>
       </c>
       <c r="E63">
-        <v>127</v>
+        <v>0.127</v>
       </c>
       <c r="F63">
         <v>0.47699999999999998</v>
@@ -34932,7 +34923,7 @@
         <v>1.6</v>
       </c>
       <c r="P63" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
@@ -34949,7 +34940,7 @@
         <v>0.159</v>
       </c>
       <c r="E64">
-        <v>127</v>
+        <v>0.127</v>
       </c>
       <c r="F64">
         <v>0.99199999999999999</v>
@@ -34982,7 +34973,7 @@
         <v>1.6</v>
       </c>
       <c r="P64" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
@@ -34999,7 +34990,7 @@
         <v>0.158</v>
       </c>
       <c r="E65">
-        <v>127</v>
+        <v>0.127</v>
       </c>
       <c r="F65">
         <v>0.98899999999999999</v>
@@ -35032,7 +35023,7 @@
         <v>1.6</v>
       </c>
       <c r="P65" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
@@ -35049,7 +35040,7 @@
         <v>0.158</v>
       </c>
       <c r="E66">
-        <v>127</v>
+        <v>0.127</v>
       </c>
       <c r="F66">
         <v>0.99399999999999999</v>
@@ -35082,7 +35073,7 @@
         <v>1.6</v>
       </c>
       <c r="P66" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
@@ -35099,7 +35090,7 @@
         <v>0.159</v>
       </c>
       <c r="E67">
-        <v>127</v>
+        <v>0.127</v>
       </c>
       <c r="F67">
         <v>1.4950000000000001</v>
@@ -35132,7 +35123,7 @@
         <v>1.7</v>
       </c>
       <c r="P67" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
@@ -35149,7 +35140,7 @@
         <v>0.158</v>
       </c>
       <c r="E68">
-        <v>127</v>
+        <v>0.127</v>
       </c>
       <c r="F68">
         <v>1.5049999999999999</v>
@@ -35182,7 +35173,7 @@
         <v>1.8</v>
       </c>
       <c r="P68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
@@ -35199,7 +35190,7 @@
         <v>0.158</v>
       </c>
       <c r="E69">
-        <v>126</v>
+        <v>0.126</v>
       </c>
       <c r="F69">
         <v>1.4990000000000001</v>
@@ -35232,7 +35223,7 @@
         <v>1.9</v>
       </c>
       <c r="P69" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
@@ -35249,7 +35240,7 @@
         <v>0.159</v>
       </c>
       <c r="E70">
-        <v>127</v>
+        <v>0.127</v>
       </c>
       <c r="F70">
         <v>2.0049999999999999</v>
@@ -35282,7 +35273,7 @@
         <v>1.7</v>
       </c>
       <c r="P70" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
@@ -35299,7 +35290,7 @@
         <v>0.158</v>
       </c>
       <c r="E71">
-        <v>126</v>
+        <v>0.126</v>
       </c>
       <c r="F71">
         <v>2.0099999999999998</v>
@@ -35332,7 +35323,7 @@
         <v>1.6</v>
       </c>
       <c r="P71" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.2">
@@ -35349,7 +35340,7 @@
         <v>0.159</v>
       </c>
       <c r="E72">
-        <v>127</v>
+        <v>0.127</v>
       </c>
       <c r="F72">
         <v>2.008</v>
@@ -35382,7 +35373,7 @@
         <v>1.6</v>
       </c>
       <c r="P72" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.2">
@@ -35399,7 +35390,7 @@
         <v>0.159</v>
       </c>
       <c r="E73">
-        <v>127</v>
+        <v>0.127</v>
       </c>
       <c r="F73">
         <v>2.4969999999999999</v>
@@ -35432,7 +35423,7 @@
         <v>1.7</v>
       </c>
       <c r="P73" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.2">
@@ -35449,7 +35440,7 @@
         <v>0.159</v>
       </c>
       <c r="E74">
-        <v>127</v>
+        <v>0.127</v>
       </c>
       <c r="F74">
         <v>2.4950000000000001</v>
@@ -35482,7 +35473,7 @@
         <v>1.7</v>
       </c>
       <c r="P74" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.2">
@@ -35499,7 +35490,7 @@
         <v>0.159</v>
       </c>
       <c r="E75">
-        <v>127</v>
+        <v>0.127</v>
       </c>
       <c r="F75">
         <v>2.496</v>
@@ -35532,7 +35523,7 @@
         <v>1.7</v>
       </c>
       <c r="P75" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -38547,7 +38538,7 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
@@ -39819,214 +39810,214 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
+      <c r="Q1" t="s">
         <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>43</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>44</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>45</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>46</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>47</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" t="s">
         <v>48</v>
       </c>
-      <c r="M2" t="s">
-        <v>48</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>49</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>50</v>
       </c>
-      <c r="P2" t="s">
-        <v>51</v>
-      </c>
       <c r="Q2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>53</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>55</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>56</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>57</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>58</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" t="s">
         <v>59</v>
       </c>
-      <c r="I3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>60</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>61</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>62</v>
-      </c>
-      <c r="M3" t="s">
-        <v>63</v>
       </c>
       <c r="N3" t="s">
         <v>22</v>
       </c>
       <c r="O3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P3" t="s">
         <v>64</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>65</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
         <v>67</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
         <v>67</v>
       </c>
-      <c r="C4" t="s">
+      <c r="H4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" t="s">
         <v>68</v>
       </c>
-      <c r="D4" t="s">
+      <c r="K4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" t="s">
+        <v>66</v>
+      </c>
+      <c r="O4" t="s">
+        <v>68</v>
+      </c>
+      <c r="P4" t="s">
         <v>69</v>
       </c>
-      <c r="E4" t="s">
+      <c r="Q4" t="s">
         <v>69</v>
-      </c>
-      <c r="F4" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J4" t="s">
-        <v>69</v>
-      </c>
-      <c r="K4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L4" t="s">
-        <v>68</v>
-      </c>
-      <c r="M4" t="s">
-        <v>68</v>
-      </c>
-      <c r="N4" t="s">
-        <v>67</v>
-      </c>
-      <c r="O4" t="s">
-        <v>69</v>
-      </c>
-      <c r="P4" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -48654,154 +48645,154 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
         <v>73</v>
-      </c>
-      <c r="B5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
         <v>76</v>
-      </c>
-      <c r="B7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
         <v>78</v>
-      </c>
-      <c r="B8" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
         <v>80</v>
-      </c>
-      <c r="B9" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
         <v>82</v>
-      </c>
-      <c r="B10" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
         <v>85</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>86</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>87</v>
-      </c>
-      <c r="D13" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" t="s">
         <v>89</v>
-      </c>
-      <c r="D14" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
         <v>91</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>92</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>93</v>
-      </c>
-      <c r="D15" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" t="s">
         <v>95</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>96</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>97</v>
-      </c>
-      <c r="D16" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" t="s">
         <v>99</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" t="s">
         <v>100</v>
-      </c>
-      <c r="C17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" t="s">
         <v>102</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" t="s">
         <v>103</v>
-      </c>
-      <c r="C18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" t="s">
         <v>105</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" t="s">
         <v>106</v>
-      </c>
-      <c r="C19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.2">
@@ -48809,67 +48800,67 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" t="s">
         <v>108</v>
-      </c>
-      <c r="C20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" t="s">
         <v>110</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" t="s">
         <v>111</v>
-      </c>
-      <c r="C21" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" t="s">
         <v>113</v>
       </c>
-      <c r="B22" t="s">
-        <v>114</v>
-      </c>
       <c r="C22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" t="s">
         <v>115</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" t="s">
         <v>116</v>
       </c>
-      <c r="C23" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="S23" t="s">
         <v>117</v>
-      </c>
-      <c r="S23" t="s">
-        <v>118</v>
       </c>
       <c r="T23" s="5"/>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" t="s">
         <v>119</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>120</v>
-      </c>
-      <c r="C24" t="s">
-        <v>121</v>
       </c>
       <c r="D24">
         <v>19</v>
@@ -48938,10 +48929,10 @@
         <v>18</v>
       </c>
       <c r="S26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T26" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U26">
         <v>19</v>
@@ -48979,100 +48970,100 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" t="s">
         <v>123</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>124</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>125</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>126</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>127</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>128</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>129</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>130</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>131</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>132</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>133</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>134</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>135</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>136</v>
-      </c>
-      <c r="O27" t="s">
-        <v>137</v>
       </c>
       <c r="P27" t="s">
         <v>5</v>
       </c>
       <c r="Q27" t="s">
+        <v>137</v>
+      </c>
+      <c r="R27" t="s">
         <v>138</v>
       </c>
-      <c r="R27" t="s">
+      <c r="S27" t="s">
         <v>139</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="T27" s="5" t="s">
+      <c r="U27" t="s">
         <v>141</v>
       </c>
-      <c r="U27" t="s">
+      <c r="V27" t="s">
         <v>142</v>
       </c>
-      <c r="V27" t="s">
+      <c r="W27" t="s">
         <v>143</v>
       </c>
-      <c r="W27" t="s">
+      <c r="X27" t="s">
         <v>144</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Y27" t="s">
         <v>145</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="Z27" t="s">
         <v>146</v>
       </c>
-      <c r="Z27" t="s">
+      <c r="AA27" t="s">
         <v>147</v>
       </c>
-      <c r="AA27" t="s">
+      <c r="AB27" t="s">
         <v>148</v>
       </c>
-      <c r="AB27" t="s">
+      <c r="AC27" t="s">
         <v>149</v>
       </c>
-      <c r="AC27" t="s">
+      <c r="AD27" t="s">
         <v>150</v>
       </c>
-      <c r="AD27" t="s">
+      <c r="AE27" t="s">
         <v>151</v>
       </c>
-      <c r="AE27" t="s">
-        <v>152</v>
-      </c>
       <c r="AF27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.2">
@@ -49086,7 +49077,7 @@
         <v>0.627</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -49172,7 +49163,7 @@
         <v>4.5</v>
       </c>
       <c r="AF28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.2">
@@ -49186,7 +49177,7 @@
         <v>0.47699999999999998</v>
       </c>
       <c r="D29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -49272,7 +49263,7 @@
         <v>4.5</v>
       </c>
       <c r="AF29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.2">
@@ -49286,7 +49277,7 @@
         <v>0.37</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -49372,7 +49363,7 @@
         <v>4.5</v>
       </c>
       <c r="AF30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.2">
@@ -49386,7 +49377,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="D31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -49472,7 +49463,7 @@
         <v>4.5</v>
       </c>
       <c r="AF31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.2">
@@ -49486,7 +49477,7 @@
         <v>0.84399999999999997</v>
       </c>
       <c r="D32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -49572,7 +49563,7 @@
         <v>4.5</v>
       </c>
       <c r="AF32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.2">
@@ -49586,7 +49577,7 @@
         <v>0.57399999999999995</v>
       </c>
       <c r="D33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -49672,7 +49663,7 @@
         <v>4.5</v>
       </c>
       <c r="AF33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.2">
@@ -49686,7 +49677,7 @@
         <v>0.63500000000000001</v>
       </c>
       <c r="D34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -49772,7 +49763,7 @@
         <v>4.5</v>
       </c>
       <c r="AF34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.2">
@@ -49786,7 +49777,7 @@
         <v>0.375</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -49872,7 +49863,7 @@
         <v>4.5</v>
       </c>
       <c r="AF35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.2">
@@ -49886,7 +49877,7 @@
         <v>0.90800000000000003</v>
       </c>
       <c r="D36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -49972,7 +49963,7 @@
         <v>4.5</v>
       </c>
       <c r="AF36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:32" x14ac:dyDescent="0.2">
@@ -49986,7 +49977,7 @@
         <v>0.246</v>
       </c>
       <c r="D37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -50072,7 +50063,7 @@
         <v>4.5</v>
       </c>
       <c r="AF37" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:32" x14ac:dyDescent="0.2">
@@ -50086,7 +50077,7 @@
         <v>0.92100000000000004</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -50172,7 +50163,7 @@
         <v>4.5</v>
       </c>
       <c r="AF38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:32" x14ac:dyDescent="0.2">
@@ -50186,7 +50177,7 @@
         <v>0.76100000000000001</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -50272,7 +50263,7 @@
         <v>4.5</v>
       </c>
       <c r="AF39" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:32" x14ac:dyDescent="0.2">
@@ -50286,7 +50277,7 @@
         <v>0.26500000000000001</v>
       </c>
       <c r="D40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -50372,7 +50363,7 @@
         <v>4.5</v>
       </c>
       <c r="AF40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.2">
@@ -50386,7 +50377,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="D41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -50472,7 +50463,7 @@
         <v>4.5</v>
       </c>
       <c r="AF41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="1:32" x14ac:dyDescent="0.2">
@@ -50486,7 +50477,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="D42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -50572,7 +50563,7 @@
         <v>4.5</v>
       </c>
       <c r="AF42" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.2">
@@ -50586,7 +50577,7 @@
         <v>0.99299999999999999</v>
       </c>
       <c r="D43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -50672,7 +50663,7 @@
         <v>4.5</v>
       </c>
       <c r="AF43" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.2">
@@ -50686,7 +50677,7 @@
         <v>0.69199999999999995</v>
       </c>
       <c r="D44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -50772,7 +50763,7 @@
         <v>4.5</v>
       </c>
       <c r="AF44" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.2">
@@ -50786,7 +50777,7 @@
         <v>0.51800000000000002</v>
       </c>
       <c r="D45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -50872,7 +50863,7 @@
         <v>4.5</v>
       </c>
       <c r="AF45" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.2">
@@ -50886,7 +50877,7 @@
         <v>0.22900000000000001</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -50972,7 +50963,7 @@
         <v>4.5</v>
       </c>
       <c r="AF46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.2">
@@ -50986,7 +50977,7 @@
         <v>0.433</v>
       </c>
       <c r="D47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -51072,7 +51063,7 @@
         <v>4.5</v>
       </c>
       <c r="AF47" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.2">
@@ -51086,7 +51077,7 @@
         <v>0.22800000000000001</v>
       </c>
       <c r="D48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -51172,7 +51163,7 @@
         <v>4.5</v>
       </c>
       <c r="AF48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:32" x14ac:dyDescent="0.2">
@@ -51186,7 +51177,7 @@
         <v>0.77200000000000002</v>
       </c>
       <c r="D49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -51272,7 +51263,7 @@
         <v>4.5</v>
       </c>
       <c r="AF49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:32" x14ac:dyDescent="0.2">
@@ -51286,7 +51277,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -51372,7 +51363,7 @@
         <v>4.5</v>
       </c>
       <c r="AF50" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:32" x14ac:dyDescent="0.2">
@@ -51386,7 +51377,7 @@
         <v>0.78300000000000003</v>
       </c>
       <c r="D51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -51472,7 +51463,7 @@
         <v>4.5</v>
       </c>
       <c r="AF51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:32" x14ac:dyDescent="0.2">
@@ -51486,7 +51477,7 @@
         <v>0.437</v>
       </c>
       <c r="D52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -51572,7 +51563,7 @@
         <v>4.5</v>
       </c>
       <c r="AF52" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:32" x14ac:dyDescent="0.2">
@@ -51586,7 +51577,7 @@
         <v>0.91900000000000004</v>
       </c>
       <c r="D53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -51672,7 +51663,7 @@
         <v>4.5</v>
       </c>
       <c r="AF53" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.2">
@@ -51686,7 +51677,7 @@
         <v>0.70499999999999996</v>
       </c>
       <c r="D54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -51772,7 +51763,7 @@
         <v>4.5</v>
       </c>
       <c r="AF54" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="55" spans="1:32" x14ac:dyDescent="0.2">
@@ -51786,7 +51777,7 @@
         <v>0.54500000000000004</v>
       </c>
       <c r="D55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -51872,7 +51863,7 @@
         <v>4.5</v>
       </c>
       <c r="AF55" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" spans="1:32" x14ac:dyDescent="0.2">
@@ -51886,7 +51877,7 @@
         <v>0.221</v>
       </c>
       <c r="D56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -51972,7 +51963,7 @@
         <v>4.5</v>
       </c>
       <c r="AF56" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finally added 2014 sensor data and updated depths for 2014 lake sample grabs
</commit_message>
<xml_diff>
--- a/01_raw data/2014_Manual_Sonde_Casts.xlsx
+++ b/01_raw data/2014_Manual_Sonde_Casts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinkincaid/ownCloud/bree_frozeN/01_raw data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C5AF90-B9A8-5141-B253-35C140097C6C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EC50EC-BBA7-EE48-89BE-F2C2FD1016DD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="840" windowWidth="31120" windowHeight="21860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2560" yWindow="840" windowWidth="31120" windowHeight="21860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All winter" sheetId="24" r:id="rId1"/>
@@ -990,7 +990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A1A403-6B98-E249-87E8-2E96DF31FB04}">
   <dimension ref="A1:P238"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -31775,7 +31775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P75"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E58" sqref="E58:E75"/>
     </sheetView>
   </sheetViews>
@@ -40188,9 +40188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:O49"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>